<commit_message>
added plots and plotting script
</commit_message>
<xml_diff>
--- a/excel_outputs/formatted_annot_manual.xlsx
+++ b/excel_outputs/formatted_annot_manual.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kzammit\Repos\rs_detector\excel_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926B1B58-5641-49C5-847D-BF0E08C9CCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102DCD23-EBD7-4CC5-90E3-CA6A56AC1D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1372</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5490" uniqueCount="1776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="1776">
   <si>
     <t>site_name</t>
   </si>
@@ -5752,7 +5755,7 @@
   <dimension ref="A1:H1372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30796,6 +30799,9 @@
       <c r="G963" t="s">
         <v>755</v>
       </c>
+      <c r="H963" t="s">
+        <v>1772</v>
+      </c>
     </row>
     <row r="964" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A964" t="s">
@@ -31053,6 +31059,9 @@
       <c r="G973" t="s">
         <v>763</v>
       </c>
+      <c r="H973" t="s">
+        <v>1772</v>
+      </c>
     </row>
     <row r="974" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A974" t="s">
@@ -41429,6 +41438,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1372" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>